<commit_message>
refactor: use a new lib to read xlsx
</commit_message>
<xml_diff>
--- a/public/ajuda-saude-cupom-template.xlsx
+++ b/public/ajuda-saude-cupom-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12345"/>
+    <workbookView windowWidth="13725" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>CODIGO DO CUPOM</t>
   </si>
@@ -38,17 +38,57 @@
   </si>
   <si>
     <t>PLANO</t>
+  </si>
+  <si>
+    <t>TIPO DE PLANO</t>
+  </si>
+  <si>
+    <t>PROMO</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>31/12/2021</t>
+  </si>
+  <si>
+    <t>Trimestral</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>UNICO</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Talvez</t>
+  </si>
+  <si>
+    <t>tres</t>
+  </si>
+  <si>
+    <t>01/99/2000</t>
+  </si>
+  <si>
+    <t>Bienal</t>
+  </si>
+  <si>
+    <t>Coletivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -67,6 +107,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,8 +123,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -84,36 +154,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,6 +184,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -152,29 +216,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -183,7 +231,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,16 +244,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,181 +260,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,6 +461,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,21 +543,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -519,12 +559,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -534,134 +574,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -671,11 +711,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -996,13 +1039,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="20.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="13.8571428571429" style="2" customWidth="1"/>
@@ -1010,34 +1053,94 @@
     <col min="4" max="4" width="27.5714285714286" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.5714285714286" style="2" customWidth="1"/>
     <col min="6" max="6" width="19.2857142857143" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.8571428571429" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.7142857142857" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.8571428571429" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.8571428571429" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5714285714286" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:8">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:9">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>